<commit_message>
feat: Completed Module 3 and started Module 4
</commit_message>
<xml_diff>
--- a/Courses/ITEC-1003/Modules/Timeline/Timeline_Buchanan1003.xlsx
+++ b/Courses/ITEC-1003/Modules/Timeline/Timeline_Buchanan1003.xlsx
@@ -491,7 +491,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border/>
     <border>
       <bottom style="thin">
@@ -503,6 +503,20 @@
       <right/>
       <top/>
       <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left/>
@@ -580,16 +594,16 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -602,7 +616,7 @@
     <xf borderId="0" fillId="7" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="7" fontId="7" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -610,11 +624,8 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="7" fontId="8" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="7" fontId="8" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="8" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
@@ -622,15 +633,18 @@
     <xf borderId="2" fillId="6" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="6" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="6" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1939,7 +1953,7 @@
       <c r="F61" s="39">
         <v>45156.0</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="29">
         <v>45149.0</v>
       </c>
       <c r="H61" s="30">
@@ -2014,12 +2028,14 @@
         <v>1.0</v>
       </c>
       <c r="E65" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="10"/>
       <c r="H65" s="16"/>
-      <c r="I65" s="17"/>
+      <c r="I65" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J65" s="18"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
@@ -2044,13 +2060,17 @@
         <v>1.0</v>
       </c>
       <c r="E67" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" s="38">
         <v>45161.0</v>
       </c>
-      <c r="G67" s="10"/>
-      <c r="H67" s="16"/>
+      <c r="G67" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H67" s="34">
+        <v>1.0</v>
+      </c>
       <c r="I67" s="17"/>
       <c r="J67" s="18"/>
     </row>
@@ -2063,11 +2083,15 @@
         <v>2.0</v>
       </c>
       <c r="E68" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="22"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="16"/>
+      <c r="G68" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H68" s="34">
+        <v>2.0</v>
+      </c>
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
     </row>
@@ -2093,14 +2117,18 @@
         <v>2.0</v>
       </c>
       <c r="E70" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="38">
         <v>45163.0</v>
       </c>
-      <c r="G70" s="10"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="17"/>
+      <c r="G70" s="27">
+        <v>45150.0</v>
+      </c>
+      <c r="H70" s="34"/>
+      <c r="I70" s="35">
+        <v>3.0</v>
+      </c>
       <c r="J70" s="18"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -2112,12 +2140,14 @@
         <v>1.0</v>
       </c>
       <c r="E71" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="10"/>
       <c r="H71" s="16"/>
-      <c r="I71" s="17"/>
+      <c r="I71" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J71" s="18"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -2142,14 +2172,18 @@
         <v>1.0</v>
       </c>
       <c r="E73" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="38">
         <v>45163.0</v>
       </c>
-      <c r="G73" s="10"/>
+      <c r="G73" s="27">
+        <v>45153.0</v>
+      </c>
       <c r="H73" s="16"/>
-      <c r="I73" s="17"/>
+      <c r="I73" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J73" s="18"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
@@ -2161,12 +2195,14 @@
         <v>1.0</v>
       </c>
       <c r="E74" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" s="22"/>
       <c r="G74" s="10"/>
       <c r="H74" s="16"/>
-      <c r="I74" s="17"/>
+      <c r="I74" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J74" s="18"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -2178,12 +2214,14 @@
         <v>1.0</v>
       </c>
       <c r="E75" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="22"/>
       <c r="G75" s="10"/>
       <c r="H75" s="16"/>
-      <c r="I75" s="17"/>
+      <c r="I75" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J75" s="18"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
@@ -2208,13 +2246,17 @@
         <v>1.0</v>
       </c>
       <c r="E77" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" s="38">
         <v>45167.0</v>
       </c>
-      <c r="G77" s="10"/>
-      <c r="H77" s="16"/>
+      <c r="G77" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H77" s="34">
+        <v>1.0</v>
+      </c>
       <c r="I77" s="17"/>
       <c r="J77" s="18"/>
     </row>
@@ -2227,12 +2269,16 @@
         <v>1.0</v>
       </c>
       <c r="E78" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="22"/>
-      <c r="G78" s="10"/>
+      <c r="G78" s="27">
+        <v>45154.0</v>
+      </c>
       <c r="H78" s="16"/>
-      <c r="I78" s="17"/>
+      <c r="I78" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J78" s="18"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
@@ -2244,12 +2290,18 @@
         <v>1.0</v>
       </c>
       <c r="E79" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="22"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="17"/>
+      <c r="G79" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H79" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="I79" s="35">
+        <v>1.0</v>
+      </c>
       <c r="J79" s="18"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
@@ -2274,14 +2326,18 @@
         <v>1.5</v>
       </c>
       <c r="E81" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" s="38">
         <v>45168.0</v>
       </c>
-      <c r="G81" s="10"/>
+      <c r="G81" s="27">
+        <v>45154.0</v>
+      </c>
       <c r="H81" s="16"/>
-      <c r="I81" s="17"/>
+      <c r="I81" s="35">
+        <v>1.5</v>
+      </c>
       <c r="J81" s="18"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -2293,12 +2349,18 @@
         <v>1.5</v>
       </c>
       <c r="E82" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="22"/>
-      <c r="G82" s="10"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="17"/>
+      <c r="G82" s="27">
+        <v>45156.0</v>
+      </c>
+      <c r="H82" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="I82" s="35">
+        <v>0.5</v>
+      </c>
       <c r="J82" s="18"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -2323,13 +2385,17 @@
         <v>1.0</v>
       </c>
       <c r="E84" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" s="38">
         <v>45170.0</v>
       </c>
-      <c r="G84" s="10"/>
-      <c r="H84" s="16"/>
+      <c r="G84" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H84" s="34">
+        <v>0.5</v>
+      </c>
       <c r="I84" s="17"/>
       <c r="J84" s="18"/>
     </row>
@@ -2342,11 +2408,15 @@
         <v>1.0</v>
       </c>
       <c r="E85" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" s="22"/>
-      <c r="G85" s="10"/>
-      <c r="H85" s="16"/>
+      <c r="G85" s="27">
+        <v>45155.0</v>
+      </c>
+      <c r="H85" s="34">
+        <v>0.5</v>
+      </c>
       <c r="I85" s="17"/>
       <c r="J85" s="18"/>
     </row>
@@ -2359,11 +2429,13 @@
         <v>1.0</v>
       </c>
       <c r="E86" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="22"/>
       <c r="G86" s="10"/>
-      <c r="H86" s="16"/>
+      <c r="H86" s="34">
+        <v>0.5</v>
+      </c>
       <c r="I86" s="17"/>
       <c r="J86" s="18"/>
     </row>
@@ -2374,23 +2446,25 @@
         <v>43</v>
       </c>
       <c r="E87" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="43">
         <v>45170.0</v>
       </c>
-      <c r="G87" s="44"/>
+      <c r="G87" s="27">
+        <v>45156.0</v>
+      </c>
       <c r="H87" s="30">
         <f t="shared" ref="H87:I87" si="2">SUM(H64:H86)</f>
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="I87" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J87" s="32">
         <f>SUM(H87:I87)</f>
-        <v>2</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
@@ -2431,7 +2505,7 @@
       <c r="E90" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F90" s="45">
+      <c r="F90" s="44">
         <v>45170.0</v>
       </c>
       <c r="G90" s="10"/>
@@ -2444,7 +2518,7 @@
       <c r="C91" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D91" s="46">
+      <c r="D91" s="45">
         <v>0.25</v>
       </c>
       <c r="E91" s="1" t="b">
@@ -2548,7 +2622,9 @@
       <c r="F97" s="38">
         <v>45175.0</v>
       </c>
-      <c r="G97" s="10"/>
+      <c r="G97" s="27">
+        <v>45155.0</v>
+      </c>
       <c r="H97" s="16"/>
       <c r="I97" s="17"/>
       <c r="J97" s="18"/>
@@ -2831,7 +2907,7 @@
       <c r="F114" s="39">
         <v>45181.0</v>
       </c>
-      <c r="G114" s="44"/>
+      <c r="G114" s="46"/>
       <c r="H114" s="30">
         <f t="shared" ref="H114:I114" si="3">SUM(H90:H113)</f>
         <v>0</v>
@@ -2985,7 +3061,7 @@
         <f>F3</f>
         <v>45184</v>
       </c>
-      <c r="G123" s="44"/>
+      <c r="G123" s="46"/>
       <c r="H123" s="30">
         <f t="shared" ref="H123:I123" si="4">SUM(H117:H122)</f>
         <v>0</v>

</xml_diff>

<commit_message>
feat: Completed Module 4 and began studying for certification
</commit_message>
<xml_diff>
--- a/Courses/ITEC-1003/Modules/Timeline/Timeline_Buchanan1003.xlsx
+++ b/Courses/ITEC-1003/Modules/Timeline/Timeline_Buchanan1003.xlsx
@@ -396,7 +396,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -445,6 +445,16 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF262626"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color rgb="FF262626"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -530,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -633,8 +643,14 @@
     <xf borderId="2" fillId="6" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -645,6 +661,9 @@
     <xf borderId="4" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="6" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2503,13 +2522,17 @@
         <v>0.25</v>
       </c>
       <c r="E90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" s="44">
         <v>45170.0</v>
       </c>
-      <c r="G90" s="10"/>
-      <c r="H90" s="16"/>
+      <c r="G90" s="27">
+        <v>45156.0</v>
+      </c>
+      <c r="H90" s="34">
+        <v>3.0</v>
+      </c>
       <c r="I90" s="17"/>
       <c r="J90" s="18"/>
     </row>
@@ -2522,7 +2545,7 @@
         <v>0.25</v>
       </c>
       <c r="E91" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="10"/>
       <c r="H91" s="16"/>
@@ -2538,7 +2561,7 @@
         <v>0.5</v>
       </c>
       <c r="E92" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" s="22"/>
       <c r="G92" s="10"/>
@@ -2555,7 +2578,7 @@
         <v>2.0</v>
       </c>
       <c r="E93" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="22"/>
       <c r="G93" s="10"/>
@@ -2585,13 +2608,17 @@
         <v>3.0</v>
       </c>
       <c r="E95" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95" s="38">
         <v>45174.0</v>
       </c>
-      <c r="G95" s="10"/>
-      <c r="H95" s="16"/>
+      <c r="G95" s="27">
+        <v>45156.0</v>
+      </c>
+      <c r="H95" s="34">
+        <v>2.0</v>
+      </c>
       <c r="I95" s="17"/>
       <c r="J95" s="18"/>
     </row>
@@ -2617,16 +2644,18 @@
         <v>1.0</v>
       </c>
       <c r="E97" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" s="38">
         <v>45175.0</v>
       </c>
-      <c r="G97" s="27">
-        <v>45155.0</v>
-      </c>
-      <c r="H97" s="16"/>
-      <c r="I97" s="17"/>
+      <c r="G97" s="46">
+        <v>45169.0</v>
+      </c>
+      <c r="H97" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="I97" s="48"/>
       <c r="J97" s="18"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
@@ -2638,11 +2667,13 @@
         <v>1.0</v>
       </c>
       <c r="E98" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="22"/>
       <c r="G98" s="10"/>
-      <c r="H98" s="16"/>
+      <c r="H98" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I98" s="17"/>
       <c r="J98" s="18"/>
     </row>
@@ -2655,11 +2686,13 @@
         <v>0.5</v>
       </c>
       <c r="E99" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" s="22"/>
       <c r="G99" s="10"/>
-      <c r="H99" s="16"/>
+      <c r="H99" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I99" s="17"/>
       <c r="J99" s="18"/>
     </row>
@@ -2672,11 +2705,13 @@
         <v>0.5</v>
       </c>
       <c r="E100" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="22"/>
       <c r="G100" s="10"/>
-      <c r="H100" s="16"/>
+      <c r="H100" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I100" s="17"/>
       <c r="J100" s="18"/>
     </row>
@@ -2702,13 +2737,15 @@
         <v>0.5</v>
       </c>
       <c r="E102" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102" s="27">
         <v>45177.0</v>
       </c>
       <c r="G102" s="10"/>
-      <c r="H102" s="16"/>
+      <c r="H102" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I102" s="17"/>
       <c r="J102" s="18"/>
     </row>
@@ -2721,11 +2758,13 @@
         <v>0.5</v>
       </c>
       <c r="E103" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="22"/>
       <c r="G103" s="10"/>
-      <c r="H103" s="16"/>
+      <c r="H103" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I103" s="17"/>
       <c r="J103" s="18"/>
     </row>
@@ -2738,11 +2777,13 @@
         <v>0.5</v>
       </c>
       <c r="E104" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="10"/>
-      <c r="H104" s="16"/>
+      <c r="H104" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I104" s="17"/>
       <c r="J104" s="18"/>
     </row>
@@ -2755,11 +2796,15 @@
         <v>1.0</v>
       </c>
       <c r="E105" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" s="22"/>
-      <c r="G105" s="10"/>
-      <c r="H105" s="16"/>
+      <c r="G105" s="46">
+        <v>45169.0</v>
+      </c>
+      <c r="H105" s="47">
+        <v>0.75</v>
+      </c>
       <c r="I105" s="17"/>
       <c r="J105" s="18"/>
     </row>
@@ -2772,11 +2817,13 @@
         <v>0.5</v>
       </c>
       <c r="E106" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" s="22"/>
       <c r="G106" s="10"/>
-      <c r="H106" s="16"/>
+      <c r="H106" s="34">
+        <v>0.5</v>
+      </c>
       <c r="I106" s="17"/>
       <c r="J106" s="18"/>
     </row>
@@ -2802,13 +2849,17 @@
         <v>3.0</v>
       </c>
       <c r="E108" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" s="38">
         <v>45177.0</v>
       </c>
-      <c r="G108" s="10"/>
-      <c r="H108" s="16"/>
+      <c r="G108" s="46">
+        <v>45169.0</v>
+      </c>
+      <c r="H108" s="34">
+        <v>0.75</v>
+      </c>
       <c r="I108" s="17"/>
       <c r="J108" s="18"/>
     </row>
@@ -2834,13 +2885,17 @@
         <v>0.5</v>
       </c>
       <c r="E110" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" s="38">
         <v>45181.0</v>
       </c>
-      <c r="G110" s="10"/>
-      <c r="H110" s="16"/>
+      <c r="G110" s="46">
+        <v>45169.0</v>
+      </c>
+      <c r="H110" s="34">
+        <v>0.1</v>
+      </c>
       <c r="I110" s="17"/>
       <c r="J110" s="18"/>
     </row>
@@ -2853,11 +2908,13 @@
         <v>1.0</v>
       </c>
       <c r="E111" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="22"/>
       <c r="G111" s="10"/>
-      <c r="H111" s="16"/>
+      <c r="H111" s="34">
+        <v>0.25</v>
+      </c>
       <c r="I111" s="17"/>
       <c r="J111" s="18"/>
     </row>
@@ -2870,11 +2927,13 @@
         <v>1.0</v>
       </c>
       <c r="E112" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" s="22"/>
       <c r="G112" s="10"/>
-      <c r="H112" s="16"/>
+      <c r="H112" s="34">
+        <v>0.1</v>
+      </c>
       <c r="I112" s="17"/>
       <c r="J112" s="18"/>
     </row>
@@ -2887,7 +2946,7 @@
         <v>0.5</v>
       </c>
       <c r="E113" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" s="22"/>
       <c r="G113" s="10"/>
@@ -2902,15 +2961,17 @@
         <v>43</v>
       </c>
       <c r="E114" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F114" s="39">
         <v>45181.0</v>
       </c>
-      <c r="G114" s="46"/>
+      <c r="G114" s="46">
+        <v>45169.0</v>
+      </c>
       <c r="H114" s="30">
         <f t="shared" ref="H114:I114" si="3">SUM(H90:H113)</f>
-        <v>0</v>
+        <v>9.7</v>
       </c>
       <c r="I114" s="31">
         <f t="shared" si="3"/>
@@ -2918,7 +2979,7 @@
       </c>
       <c r="J114" s="32">
         <f>SUM(H114:I114)</f>
-        <v>0</v>
+        <v>9.7</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
@@ -2959,7 +3020,7 @@
       <c r="E117" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F117" s="47">
+      <c r="F117" s="49">
         <v>45182.0</v>
       </c>
       <c r="G117" s="10"/>
@@ -3047,21 +3108,21 @@
       <c r="J122" s="18"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="B123" s="48"/>
-      <c r="C123" s="49" t="s">
+      <c r="B123" s="50"/>
+      <c r="C123" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="D123" s="50">
+      <c r="D123" s="52">
         <v>1.0</v>
       </c>
       <c r="E123" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F123" s="51">
+      <c r="F123" s="53">
         <f>F3</f>
         <v>45184</v>
       </c>
-      <c r="G123" s="46"/>
+      <c r="G123" s="54"/>
       <c r="H123" s="30">
         <f t="shared" ref="H123:I123" si="4">SUM(H117:H122)</f>
         <v>0</v>

</xml_diff>